<commit_message>
updated documents, added venue information
</commit_message>
<xml_diff>
--- a/2022_Symposium/File_&_Task_INDEX.xlsx
+++ b/2022_Symposium/File_&_Task_INDEX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e284e911/Documents/GitHub/KUGC_SymposiumPlanning/2022_Symposium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11952D6-5B07-1E42-8DBB-1C5DA8F3E10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9ACA8A-B328-8848-8CED-EE78DF0D4586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35840" yWindow="460" windowWidth="35840" windowHeight="21140" xr2:uid="{61BACC42-D555-0743-B8D5-ED3775F296E7}"/>
+    <workbookView xWindow="-300" yWindow="460" windowWidth="35840" windowHeight="18320" xr2:uid="{61BACC42-D555-0743-B8D5-ED3775F296E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="219">
   <si>
     <t>Venue picked and date reserved</t>
   </si>
@@ -1623,9 +1623,6 @@
     </r>
   </si>
   <si>
-    <t>Poster judging preliminary results</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1741,9 +1738,6 @@
     </r>
   </si>
   <si>
-    <t>All submitted talk abstracts and voting</t>
-  </si>
-  <si>
     <t>Registration tables, vendor tables, posters, presentation podium, screen, light control, coffee/tea area, buffet area,</t>
   </si>
   <si>
@@ -1793,6 +1787,58 @@
         <scheme val="minor"/>
       </rPr>
       <t>Pumping_Station.docx</t>
+    </r>
+  </si>
+  <si>
+    <t>Poster judging template</t>
+  </si>
+  <si>
+    <t>All submitted talk abstracts</t>
+  </si>
+  <si>
+    <t>Checklist of items for venue and food</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2022_Symposium/General_Information/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Generic_Venue_Checklist_060722.docx</t>
+    </r>
+  </si>
+  <si>
+    <t>Email to venue to initate planning</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2022_Symposium/Email_Templates/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Generic_Initial_Venue_Correspondence_060722.docx</t>
     </r>
   </si>
 </sst>
@@ -2187,10 +2233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068BB468-CC10-4B43-A335-808C81961EAE}">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B93" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="B81" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2291,7 +2337,7 @@
         <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2946,7 +2992,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B90" t="s">
         <v>135</v>
@@ -2967,354 +3013,371 @@
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="C92" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
       <c r="B93" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
       <c r="B94" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C94" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
       <c r="B95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C95" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C96" t="s">
-        <v>143</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
+      <c r="B97" t="s">
+        <v>142</v>
+      </c>
+      <c r="C97" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>145</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
-        <v>146</v>
-      </c>
-      <c r="C99" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C100" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C101" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>152</v>
+        <v>215</v>
       </c>
       <c r="C102" t="s">
-        <v>153</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C103" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C104" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C105" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C106" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C107" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C108" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C109" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="C110" t="s">
-        <v>214</v>
+        <v>31</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C111" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="C112" t="s">
-        <v>42</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C113" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
+        <v>171</v>
+      </c>
+      <c r="C114" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>172</v>
+      </c>
+      <c r="C115" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
         <v>173</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C116" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B118" t="s">
         <v>176</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C118" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B117" t="s">
-        <v>177</v>
-      </c>
-      <c r="C117" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
-        <v>179</v>
-      </c>
-      <c r="C118" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="C119" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C120" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="C121" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
+        <v>181</v>
+      </c>
+      <c r="C122" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B123" t="s">
+        <v>183</v>
+      </c>
+      <c r="C123" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
         <v>184</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C124" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B124" t="s">
-        <v>186</v>
-      </c>
-      <c r="C124" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B126" t="s">
+        <v>186</v>
+      </c>
+      <c r="C126" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>188</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C128" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B127" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
         <v>190</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="3" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>193</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C131" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B130" t="s">
-        <v>195</v>
-      </c>
-      <c r="C130" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B131" t="s">
-        <v>211</v>
-      </c>
-      <c r="C131" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C132" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
+        <v>209</v>
+      </c>
+      <c r="C133" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>213</v>
+      </c>
+      <c r="C134" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B135" t="s">
+        <v>198</v>
+      </c>
+      <c r="C135" t="s">
         <v>199</v>
       </c>
-      <c r="C133" t="s">
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
+      <c r="B137" t="s">
         <v>201</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C137" t="s">
         <v>202</v>
-      </c>
-      <c r="C135" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B136" t="s">
-        <v>204</v>
-      </c>
-      <c r="C136" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B137" t="s">
-        <v>206</v>
-      </c>
-      <c r="C137" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C138" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B139" t="s">
+        <v>205</v>
+      </c>
+      <c r="C139" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
+        <v>214</v>
+      </c>
+      <c r="C140" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>